<commit_message>
fix: let original SOP circuits not having complement SOPs
</commit_message>
<xml_diff>
--- a/SASIMI-VECBEE/result/benchmark-information/benchmark-information.xlsx
+++ b/SASIMI-VECBEE/result/benchmark-information/benchmark-information.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -136,10 +136,10 @@
     <t>MAC</t>
   </si>
   <si>
-    <t>48/33</t>
-  </si>
-  <si>
-    <t>8-bit multiplier and accumulator</t>
+    <t>32/17</t>
+  </si>
+  <si>
+    <t>multiplier and accumulator</t>
   </si>
   <si>
     <t>EUDIST</t>
@@ -148,13 +148,16 @@
     <t>32/16</t>
   </si>
   <si>
-    <t>8-bit Euclidean distance unit</t>
+    <t>Euclidean distance unit</t>
   </si>
   <si>
     <t>SAD</t>
   </si>
   <si>
-    <t>8-bit sum of absolute differences</t>
+    <t>48/13</t>
+  </si>
+  <si>
+    <t>sum of absolute differences</t>
   </si>
 </sst>
 </file>
@@ -162,10 +165,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -186,66 +189,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -260,22 +203,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -283,9 +210,54 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -299,6 +271,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -308,13 +318,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -329,18 +332,108 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -353,85 +446,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -443,73 +512,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -523,17 +526,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -549,26 +546,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -605,6 +582,32 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -625,142 +628,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1105,7 +1108,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75" outlineLevelCol="6"/>
@@ -1423,16 +1426,16 @@
         <v>41</v>
       </c>
       <c r="D14">
-        <v>583</v>
+        <v>560</v>
       </c>
       <c r="E14">
-        <v>1454</v>
+        <v>1351</v>
       </c>
       <c r="F14" s="2">
-        <v>1447</v>
+        <v>1372</v>
       </c>
       <c r="G14" s="2">
-        <v>78.8</v>
+        <v>57.5</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1463,22 +1466,22 @@
         <v>45</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D16">
-        <v>412</v>
+        <v>425</v>
       </c>
       <c r="E16">
-        <v>1019</v>
+        <v>962</v>
       </c>
       <c r="F16" s="2">
-        <v>908</v>
+        <v>999</v>
       </c>
       <c r="G16" s="2">
-        <v>52.9</v>
+        <v>70.9</v>
       </c>
     </row>
     <row r="24" spans="4:5">

</xml_diff>

<commit_message>
test: experimental results of epfl
</commit_message>
<xml_diff>
--- a/SASIMI-VECBEE/result/benchmark-information/benchmark-information.xlsx
+++ b/SASIMI-VECBEE/result/benchmark-information/benchmark-information.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="94">
   <si>
     <t>Name</t>
   </si>
@@ -158,6 +158,144 @@
   </si>
   <si>
     <t>sum of absolute differences</t>
+  </si>
+  <si>
+    <t>accurate circuit</t>
+  </si>
+  <si>
+    <t>approximate circuit</t>
+  </si>
+  <si>
+    <t>Original area</t>
+  </si>
+  <si>
+    <t>Original delay</t>
+  </si>
+  <si>
+    <t>Area ratio</t>
+  </si>
+  <si>
+    <t>Delay ratio</t>
+  </si>
+  <si>
+    <t>Runtime/s</t>
+  </si>
+  <si>
+    <t>adder</t>
+  </si>
+  <si>
+    <t>256/129</t>
+  </si>
+  <si>
+    <t>arbiter</t>
+  </si>
+  <si>
+    <t>bar</t>
+  </si>
+  <si>
+    <t>135/128</t>
+  </si>
+  <si>
+    <t>cavlc</t>
+  </si>
+  <si>
+    <t>10/11</t>
+  </si>
+  <si>
+    <t>ctrl</t>
+  </si>
+  <si>
+    <t>7/26</t>
+  </si>
+  <si>
+    <t>dec</t>
+  </si>
+  <si>
+    <t>8/256</t>
+  </si>
+  <si>
+    <t>div</t>
+  </si>
+  <si>
+    <t>128/128</t>
+  </si>
+  <si>
+    <t>hyp</t>
+  </si>
+  <si>
+    <t>256/128</t>
+  </si>
+  <si>
+    <t>i2c</t>
+  </si>
+  <si>
+    <t>147/142</t>
+  </si>
+  <si>
+    <t>int2float</t>
+  </si>
+  <si>
+    <t>11/7</t>
+  </si>
+  <si>
+    <t>log</t>
+  </si>
+  <si>
+    <t>32/32</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>512/130</t>
+  </si>
+  <si>
+    <t>mem</t>
+  </si>
+  <si>
+    <t>1204/1231</t>
+  </si>
+  <si>
+    <t>multiplier</t>
+  </si>
+  <si>
+    <t>priority</t>
+  </si>
+  <si>
+    <t>128/8</t>
+  </si>
+  <si>
+    <t>router</t>
+  </si>
+  <si>
+    <t>60/30</t>
+  </si>
+  <si>
+    <t>sin</t>
+  </si>
+  <si>
+    <t>24/25</t>
+  </si>
+  <si>
+    <t>sqrt</t>
+  </si>
+  <si>
+    <t>128/64</t>
+  </si>
+  <si>
+    <t>square</t>
+  </si>
+  <si>
+    <t>64/128</t>
+  </si>
+  <si>
+    <t>voter</t>
+  </si>
+  <si>
+    <t>1001/1</t>
+  </si>
+  <si>
+    <t>average</t>
   </si>
 </sst>
 </file>
@@ -773,7 +911,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -785,6 +923,12 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFill="true" applyAlignment="true">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1105,15 +1249,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75" outlineLevelCol="7"/>
   <cols>
-    <col min="3" max="3" width="29.9" customWidth="true"/>
+    <col min="3" max="3" width="12.8" customWidth="true"/>
+    <col min="4" max="4" width="11.2" customWidth="true"/>
+    <col min="5" max="5" width="12.2" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1484,39 +1630,465 @@
         <v>70.9</v>
       </c>
     </row>
-    <row r="24" spans="4:5">
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-    </row>
-    <row r="25" spans="4:5">
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-    </row>
-    <row r="26" spans="4:5">
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="4:5">
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="4:5">
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="4:5">
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-    </row>
-    <row r="30" spans="4:5">
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-    </row>
-    <row r="31" spans="4:5">
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
+    <row r="19" spans="1:8">
+      <c r="A19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="4">
+        <v>1117</v>
+      </c>
+      <c r="D21" s="4">
+        <v>2594</v>
+      </c>
+      <c r="E21" s="4">
+        <v>303.8</v>
+      </c>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="4">
+        <v>857</v>
+      </c>
+      <c r="D22" s="4">
+        <v>1802</v>
+      </c>
+      <c r="E22" s="4">
+        <v>242.6</v>
+      </c>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="4">
+        <v>1927</v>
+      </c>
+      <c r="D23" s="4">
+        <v>5383</v>
+      </c>
+      <c r="E23" s="4">
+        <v>51.6</v>
+      </c>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="4">
+        <v>441</v>
+      </c>
+      <c r="D24" s="4">
+        <v>1093</v>
+      </c>
+      <c r="E24" s="4">
+        <v>24.2</v>
+      </c>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="4">
+        <v>87</v>
+      </c>
+      <c r="D25" s="4">
+        <v>195</v>
+      </c>
+      <c r="E25" s="4">
+        <v>12.7</v>
+      </c>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" s="4">
+        <v>433</v>
+      </c>
+      <c r="D26" s="4">
+        <v>995</v>
+      </c>
+      <c r="E26" s="4">
+        <v>29</v>
+      </c>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="4">
+        <v>17710</v>
+      </c>
+      <c r="D27" s="4">
+        <f>47469</f>
+        <v>47469</v>
+      </c>
+      <c r="E27" s="4">
+        <v>5533.8</v>
+      </c>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="4">
+        <v>278279</v>
+      </c>
+      <c r="D28" s="4">
+        <v>687703</v>
+      </c>
+      <c r="E28" s="4">
+        <v>17121.19</v>
+      </c>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" s="4">
+        <v>611</v>
+      </c>
+      <c r="D29" s="4">
+        <v>1428</v>
+      </c>
+      <c r="E29" s="4">
+        <v>31.2</v>
+      </c>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" s="4">
+        <v>147</v>
+      </c>
+      <c r="D30" s="4">
+        <v>341</v>
+      </c>
+      <c r="E30" s="4">
+        <v>19.5</v>
+      </c>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="4">
+        <v>27468</v>
+      </c>
+      <c r="D31" s="4">
+        <v>69688</v>
+      </c>
+      <c r="E31" s="4">
+        <v>651.4</v>
+      </c>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32" s="4">
+        <v>2163</v>
+      </c>
+      <c r="D32" s="4">
+        <v>5041</v>
+      </c>
+      <c r="E32" s="4">
+        <v>466.9</v>
+      </c>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" s="4">
+        <v>6205</v>
+      </c>
+      <c r="D33" s="4">
+        <v>14671</v>
+      </c>
+      <c r="E33" s="4">
+        <v>101.9</v>
+      </c>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" s="4">
+        <v>20260</v>
+      </c>
+      <c r="D34" s="4">
+        <v>54205</v>
+      </c>
+      <c r="E34" s="4">
+        <v>419.5</v>
+      </c>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C35" s="4">
+        <v>351</v>
+      </c>
+      <c r="D35" s="4">
+        <v>741</v>
+      </c>
+      <c r="E35" s="4">
+        <v>126.8</v>
+      </c>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C36" s="4">
+        <v>109</v>
+      </c>
+      <c r="D36" s="4">
+        <v>186</v>
+      </c>
+      <c r="E36" s="4">
+        <v>13.7</v>
+      </c>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C37" s="4">
+        <v>5534</v>
+      </c>
+      <c r="D37" s="4">
+        <v>13552</v>
+      </c>
+      <c r="E37" s="4">
+        <v>272.9</v>
+      </c>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C38" s="4">
+        <v>16584</v>
+      </c>
+      <c r="D38" s="4">
+        <v>43859</v>
+      </c>
+      <c r="E38" s="4">
+        <v>7304</v>
+      </c>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C39" s="4">
+        <v>14967</v>
+      </c>
+      <c r="D39" s="4">
+        <v>37672</v>
+      </c>
+      <c r="E39" s="4">
+        <v>355.5</v>
+      </c>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C40" s="4">
+        <v>14112</v>
+      </c>
+      <c r="D40" s="4">
+        <v>33683</v>
+      </c>
+      <c r="E40" s="4">
+        <v>95.8</v>
+      </c>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="A19:A20"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>